<commit_message>
Added Excel to working_docs - stores table data
</commit_message>
<xml_diff>
--- a/.working_documents/Book.xlsx
+++ b/.working_documents/Book.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="131" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05C9C59C-0137-48DF-AF1D-C04CAD081C70}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DED0CAA-BA81-46D1-A568-1D051CF1BFC5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="artist" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7491FB-632A-4E40-8479-13F986F24370}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -793,8 +793,8 @@
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>